<commit_message>
only values through /llm and for /new with other TB incorrect
</commit_message>
<xml_diff>
--- a/generated_notes_excel/notes.xlsx
+++ b/generated_notes_excel/notes.xlsx
@@ -75,11 +75,11 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
@@ -449,7 +449,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,8 +458,8 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="29" customWidth="1" min="1" max="1"/>
-    <col width="14" customWidth="1" min="2" max="2"/>
-    <col width="15" customWidth="1" min="3" max="3"/>
+    <col width="16" customWidth="1" min="2" max="2"/>
+    <col width="16" customWidth="1" min="3" max="3"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -490,38 +490,46 @@
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
         <is>
+          <t>Particulars</t>
+        </is>
+      </c>
+      <c r="B4" s="4" t="inlineStr">
+        <is>
           <t>March 31, 2024</t>
         </is>
       </c>
-      <c r="B4" s="4" t="inlineStr">
-        <is>
-          <t>330858462.82</t>
-        </is>
-      </c>
-      <c r="C4" s="4" t="inlineStr"/>
+      <c r="C4" s="4" t="inlineStr">
+        <is>
+          <t>March 31, 2023</t>
+        </is>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" s="3" t="inlineStr">
-        <is>
-          <t>March 31, 2023</t>
+      <c r="A5" s="5" t="inlineStr">
+        <is>
+          <t>Domestic</t>
         </is>
       </c>
       <c r="B5" s="4" t="inlineStr">
         <is>
+          <t>354.42</t>
+        </is>
+      </c>
+      <c r="C5" s="4" t="inlineStr">
+        <is>
           <t>0.00</t>
         </is>
       </c>
-      <c r="C5" s="4" t="inlineStr"/>
     </row>
     <row r="6">
-      <c r="A6" s="3" t="inlineStr">
-        <is>
-          <t>Domestic</t>
+      <c r="A6" s="5" t="inlineStr">
+        <is>
+          <t>Exports</t>
         </is>
       </c>
       <c r="B6" s="4" t="inlineStr">
         <is>
-          <t>25661755.00</t>
+          <t>10.00</t>
         </is>
       </c>
       <c r="C6" s="4" t="inlineStr">
@@ -533,12 +541,12 @@
     <row r="7">
       <c r="A7" s="3" t="inlineStr">
         <is>
-          <t>Exports</t>
+          <t>Total Sale of Services</t>
         </is>
       </c>
       <c r="B7" s="4" t="inlineStr">
         <is>
-          <t>305206707.82</t>
+          <t>364.42</t>
         </is>
       </c>
       <c r="C7" s="4" t="inlineStr">
@@ -547,35 +555,26 @@
         </is>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="5" t="inlineStr">
-        <is>
-          <t>Total Sale of Services</t>
-        </is>
-      </c>
-      <c r="B8" s="4" t="inlineStr">
-        <is>
-          <t>330858462.82</t>
-        </is>
-      </c>
-      <c r="C8" s="4" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-    </row>
-    <row r="9"/>
+    <row r="8"/>
+    <row r="9">
+      <c r="A9" s="6" t="inlineStr">
+        <is>
+          <t>Summary:</t>
+        </is>
+      </c>
+    </row>
     <row r="10">
-      <c r="A10" s="6" t="inlineStr">
-        <is>
-          <t>Summary:</t>
-        </is>
-      </c>
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Total Amount:</t>
+        </is>
+      </c>
+      <c r="B10" s="7" t="n"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Total Amount:</t>
+          <t>Total Amount (Lakhs):</t>
         </is>
       </c>
       <c r="B11" s="7" t="n"/>
@@ -583,18 +582,10 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Total Amount (Lakhs):</t>
+          <t>Matched Accounts Count:</t>
         </is>
       </c>
       <c r="B12" s="7" t="n"/>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Matched Accounts Count:</t>
-        </is>
-      </c>
-      <c r="B13" s="7" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
handled multiple file input at /new
</commit_message>
<xml_diff>
--- a/generated_notes_excel/notes.xlsx
+++ b/generated_notes_excel/notes.xlsx
@@ -7,7 +7,8 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="16. Revenue from Operations" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="13. Cash and Bank Balances" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="14. Short Term Loans and Advanc" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -449,7 +450,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -457,7 +458,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="29" customWidth="1" min="1" max="1"/>
+    <col width="41" customWidth="1" min="1" max="1"/>
     <col width="16" customWidth="1" min="2" max="2"/>
     <col width="16" customWidth="1" min="3" max="3"/>
   </cols>
@@ -465,7 +466,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>16. Revenue from Operations</t>
+          <t>13. Cash and Bank Balances</t>
         </is>
       </c>
     </row>
@@ -507,12 +508,12 @@
     <row r="5">
       <c r="A5" s="5" t="inlineStr">
         <is>
-          <t>Domestic</t>
+          <t>Balances with banks in current accounts</t>
         </is>
       </c>
       <c r="B5" s="4" t="inlineStr">
         <is>
-          <t>358.82</t>
+          <t>188.43</t>
         </is>
       </c>
       <c r="C5" s="4" t="inlineStr">
@@ -524,12 +525,12 @@
     <row r="6">
       <c r="A6" s="5" t="inlineStr">
         <is>
-          <t>Exports</t>
+          <t>Cash on hand</t>
         </is>
       </c>
       <c r="B6" s="4" t="inlineStr">
         <is>
-          <t>5.60</t>
+          <t>0.37</t>
         </is>
       </c>
       <c r="C6" s="4" t="inlineStr">
@@ -539,14 +540,14 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="3" t="inlineStr">
-        <is>
-          <t>Total Sale of Services</t>
+      <c r="A7" s="5" t="inlineStr">
+        <is>
+          <t>Fixed Deposits with ICICI Bank</t>
         </is>
       </c>
       <c r="B7" s="4" t="inlineStr">
         <is>
-          <t>364.42</t>
+          <t>8.14</t>
         </is>
       </c>
       <c r="C7" s="4" t="inlineStr">
@@ -555,26 +556,35 @@
         </is>
       </c>
     </row>
-    <row r="8"/>
-    <row r="9">
-      <c r="A9" s="6" t="inlineStr">
+    <row r="8">
+      <c r="A8" s="3" t="inlineStr">
+        <is>
+          <t>Total Total</t>
+        </is>
+      </c>
+      <c r="B8" s="4" t="inlineStr">
+        <is>
+          <t>192.54</t>
+        </is>
+      </c>
+      <c r="C8" s="4" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="9"/>
+    <row r="10">
+      <c r="A10" s="6" t="inlineStr">
         <is>
           <t>Summary:</t>
         </is>
       </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Total Amount:</t>
-        </is>
-      </c>
-      <c r="B10" s="7" t="n"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Total Amount (Lakhs):</t>
+          <t>Total Amount:</t>
         </is>
       </c>
       <c r="B11" s="7" t="n"/>
@@ -582,10 +592,201 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
+          <t>Total Amount (Lakhs):</t>
+        </is>
+      </c>
+      <c r="B12" s="7" t="n"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
           <t>Matched Accounts Count:</t>
         </is>
       </c>
+      <c r="B13" s="7" t="n"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="48" customWidth="1" min="1" max="1"/>
+    <col width="16" customWidth="1" min="2" max="2"/>
+    <col width="16" customWidth="1" min="3" max="3"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>14. Short Term Loans and Advances</t>
+        </is>
+      </c>
+    </row>
+    <row r="2"/>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>Particulars</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="inlineStr">
+        <is>
+          <t>Current Year</t>
+        </is>
+      </c>
+      <c r="C3" s="2" t="inlineStr">
+        <is>
+          <t>Previous Year</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="inlineStr">
+        <is>
+          <t>Particulars</t>
+        </is>
+      </c>
+      <c r="B4" s="4" t="inlineStr">
+        <is>
+          <t>March 31, 2024</t>
+        </is>
+      </c>
+      <c r="C4" s="4" t="inlineStr">
+        <is>
+          <t>March 31, 2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="5" t="inlineStr">
+        <is>
+          <t>Prepaid Expenses</t>
+        </is>
+      </c>
+      <c r="B5" s="4" t="inlineStr">
+        <is>
+          <t>15.90</t>
+        </is>
+      </c>
+      <c r="C5" s="4" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="5" t="inlineStr">
+        <is>
+          <t>Other Advances</t>
+        </is>
+      </c>
+      <c r="B6" s="4" t="inlineStr">
+        <is>
+          <t>257.02</t>
+        </is>
+      </c>
+      <c r="C6" s="4" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="5" t="inlineStr">
+        <is>
+          <t>Advance Tax</t>
+        </is>
+      </c>
+      <c r="B7" s="4" t="inlineStr">
+        <is>
+          <t>112.85</t>
+        </is>
+      </c>
+      <c r="C7" s="4" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="5" t="inlineStr">
+        <is>
+          <t>Balances with statutory/government authorities</t>
+        </is>
+      </c>
+      <c r="B8" s="4" t="inlineStr">
+        <is>
+          <t>357.96</t>
+        </is>
+      </c>
+      <c r="C8" s="4" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="3" t="inlineStr">
+        <is>
+          <t>Total Total</t>
+        </is>
+      </c>
+      <c r="B9" s="4" t="inlineStr">
+        <is>
+          <t>743.74</t>
+        </is>
+      </c>
+      <c r="C9" s="4" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="10"/>
+    <row r="11">
+      <c r="A11" s="6" t="inlineStr">
+        <is>
+          <t>Summary:</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Total Amount:</t>
+        </is>
+      </c>
       <c r="B12" s="7" t="n"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Total Amount (Lakhs):</t>
+        </is>
+      </c>
+      <c r="B13" s="7" t="n"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Matched Accounts Count:</t>
+        </is>
+      </c>
+      <c r="B14" s="7" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>